<commit_message>
CRIAÇÃO DE INTERFACE GRAFICA (GUI)
</commit_message>
<xml_diff>
--- a/relatorios_padaria/Estoque/Relatorio_de_Estoque.xlsx
+++ b/relatorios_padaria/Estoque/Relatorio_de_Estoque.xlsx
@@ -444,7 +444,7 @@
     <col width="19" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="16" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Pães</t>
+          <t>Pães e doces</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
         <v>3</v>
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>25</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
         <v>30</v>
@@ -548,7 +548,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
         <v>4.5</v>

</xml_diff>